<commit_message>
added a sheet to joseph poultry
</commit_message>
<xml_diff>
--- a/JOSEPH Poultry.xlsx
+++ b/JOSEPH Poultry.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KUREETHADOM\Common\Poultry Farm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E393AA55-7577-46D0-AE18-FC4863C5B529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8229F3E4-68C9-42A3-A4D8-465293B68ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHICKS" sheetId="1" r:id="rId1"/>
     <sheet name="EXPENSE" sheetId="4" r:id="rId2"/>
     <sheet name="SALES" sheetId="3" r:id="rId3"/>
+    <sheet name="Pending Payment" sheetId="5" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="81">
   <si>
     <t>Date of Arrival</t>
   </si>
@@ -257,6 +258,18 @@
   <si>
     <t>JOSEPH POULTRY</t>
   </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Not Paid</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
 </sst>
 </file>
 
@@ -1136,7 +1149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1208,6 +1221,10 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1605,6 +1622,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1634,6 +1654,7 @@
       <sheetName val="CHICKS"/>
       <sheetName val="EXPENSE"/>
       <sheetName val="SALES"/>
+      <sheetName val="Pending Payment"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -1660,6 +1681,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1954,7 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:G3"/>
     </sheetView>
   </sheetViews>
@@ -1969,20 +1991,20 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="72"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="73"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77"/>
     </row>
     <row r="4" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
@@ -1992,43 +2014,43 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="79"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="77"/>
+      <c r="B6" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="79"/>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="79"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="78"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="83"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="81"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="21"/>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2133,10 +2155,10 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="I17" s="66" t="s">
+      <c r="I17" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="55">
+      <c r="J17" s="57">
         <f>C74</f>
         <v>0</v>
       </c>
@@ -2160,8 +2182,8 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="56"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="58"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
       <c r="M18" s="17"/>
@@ -2204,10 +2226,10 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="I20" s="57" t="s">
+      <c r="I20" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="62">
         <f>D9-J17</f>
         <v>0</v>
       </c>
@@ -2216,10 +2238,10 @@
       <c r="M20" s="17"/>
     </row>
     <row r="21" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="84" t="s">
+      <c r="A21" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="85"/>
+      <c r="B21" s="87"/>
       <c r="C21" s="29">
         <f>SUM(C13:C20)</f>
         <v>0</v>
@@ -2235,8 +2257,8 @@
       <c r="G21" s="7">
         <v>165</v>
       </c>
-      <c r="I21" s="58"/>
-      <c r="J21" s="61"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="63"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
       <c r="M21" s="17"/>
@@ -2257,8 +2279,8 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="61"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="63"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
       <c r="M22" s="17"/>
@@ -2279,8 +2301,8 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="62"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="64"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
       <c r="M23" s="17"/>
@@ -2345,15 +2367,15 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="I26" s="57" t="s">
+      <c r="I26" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="63"/>
+      <c r="J26" s="65"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="86" t="s">
+      <c r="L26" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="M26" s="63"/>
+      <c r="M26" s="65"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
@@ -2371,11 +2393,11 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="64"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="66"/>
       <c r="K27" s="16"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="64"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="66"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
@@ -2393,17 +2415,17 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="64"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="66"/>
       <c r="K28" s="16"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="64"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="66"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="84" t="s">
+      <c r="A29" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="85"/>
+      <c r="B29" s="87"/>
       <c r="C29" s="29">
         <f>SUM(C22:C28)</f>
         <v>0</v>
@@ -2419,11 +2441,11 @@
       <c r="G29" s="7">
         <v>460</v>
       </c>
-      <c r="I29" s="58"/>
-      <c r="J29" s="64"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="66"/>
       <c r="K29" s="16"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="64"/>
+      <c r="L29" s="89"/>
+      <c r="M29" s="66"/>
     </row>
     <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8">
@@ -2441,11 +2463,11 @@
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="65"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="67"/>
       <c r="K30" s="16"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="65"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="67"/>
     </row>
     <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8">
@@ -2485,15 +2507,15 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="I32" s="57" t="s">
+      <c r="I32" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="J32" s="63"/>
+      <c r="J32" s="65"/>
       <c r="K32" s="16"/>
-      <c r="L32" s="86" t="s">
+      <c r="L32" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="M32" s="91">
+      <c r="M32" s="93">
         <f>D74-M26</f>
         <v>0</v>
       </c>
@@ -2514,11 +2536,11 @@
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="64"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="66"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="89"/>
-      <c r="M33" s="92"/>
+      <c r="L33" s="91"/>
+      <c r="M33" s="94"/>
     </row>
     <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8">
@@ -2536,11 +2558,11 @@
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="64"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="66"/>
       <c r="K34" s="16"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="93"/>
+      <c r="L34" s="92"/>
+      <c r="M34" s="95"/>
     </row>
     <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8">
@@ -2558,8 +2580,8 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="65"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="67"/>
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
       <c r="M35" s="25"/>
@@ -2583,19 +2605,19 @@
       <c r="I36" s="18"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="98" t="s">
+      <c r="L36" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="M36" s="99">
+      <c r="M36" s="101">
         <f>(((J26/1000)+J32)*J20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="84" t="s">
+      <c r="A37" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="85"/>
+      <c r="B37" s="87"/>
       <c r="C37" s="29">
         <f>SUM(C30:C36)</f>
         <v>0</v>
@@ -2614,8 +2636,8 @@
       <c r="I37" s="18"/>
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="100"/>
+      <c r="L37" s="92"/>
+      <c r="M37" s="102"/>
     </row>
     <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8">
@@ -2655,10 +2677,10 @@
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-      <c r="I39" s="101" t="s">
+      <c r="I39" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="103" t="e">
+      <c r="J39" s="105" t="e">
         <f>((50*M32)/M36)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2682,8 +2704,8 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="106"/>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
       <c r="M40" s="20"/>
@@ -2757,10 +2779,10 @@
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="84" t="s">
+      <c r="A45" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="85"/>
+      <c r="B45" s="87"/>
       <c r="C45" s="29">
         <f>SUM(C38:C44)</f>
         <v>0</v>
@@ -2897,10 +2919,10 @@
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="84" t="s">
+      <c r="A53" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="85"/>
+      <c r="B53" s="87"/>
       <c r="C53" s="29">
         <f>SUM(C46:C52)</f>
         <v>0</v>
@@ -3037,10 +3059,10 @@
       <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="84" t="s">
+      <c r="A61" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B61" s="85"/>
+      <c r="B61" s="87"/>
       <c r="C61" s="29">
         <f>SUM(C54:C60)</f>
         <v>0</v>
@@ -3189,10 +3211,10 @@
       <c r="L68" s="27"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="84" t="s">
+      <c r="A69" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B69" s="85"/>
+      <c r="B69" s="87"/>
       <c r="C69" s="29">
         <f>SUM(C62:C68)</f>
         <v>0</v>
@@ -3244,10 +3266,10 @@
       <c r="L72" s="27"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="94" t="s">
+      <c r="A73" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B73" s="95"/>
+      <c r="B73" s="97"/>
       <c r="C73" s="9" t="s">
         <v>4</v>
       </c>
@@ -3261,8 +3283,8 @@
       <c r="L73" s="27"/>
     </row>
     <row r="74" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="96"/>
-      <c r="B74" s="97"/>
+      <c r="A74" s="98"/>
+      <c r="B74" s="99"/>
       <c r="C74" s="24">
         <f>C21+C29+C37+C45+C53+C61+C69+C70+C71</f>
         <v>0</v>
@@ -3271,10 +3293,10 @@
         <f>D21+D29+D37+D45+D53+D61+D69+D70+D71</f>
         <v>0</v>
       </c>
-      <c r="I74" s="88"/>
-      <c r="J74" s="88"/>
-      <c r="K74" s="88"/>
-      <c r="L74" s="88"/>
+      <c r="I74" s="90"/>
+      <c r="J74" s="90"/>
+      <c r="K74" s="90"/>
+      <c r="L74" s="90"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I75" s="26"/>
@@ -3289,7 +3311,7 @@
       <c r="L76" s="27"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H77" s="51" t="s">
+      <c r="H77" s="53" t="s">
         <v>75</v>
       </c>
       <c r="I77" s="27"/>
@@ -3298,64 +3320,64 @@
       <c r="L77" s="27"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B78" s="105" t="s">
+      <c r="B78" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="C78" s="105" t="s">
+      <c r="C78" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="D78" s="105" t="s">
+      <c r="D78" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="E78" s="105" t="s">
+      <c r="E78" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="H78" s="51"/>
+      <c r="H78" s="53"/>
       <c r="I78" s="27"/>
       <c r="J78" s="27"/>
       <c r="K78" s="27"/>
       <c r="L78" s="27"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B79" s="105"/>
-      <c r="C79" s="105"/>
-      <c r="D79" s="105"/>
-      <c r="E79" s="105"/>
-      <c r="H79" s="51"/>
-      <c r="I79" s="53"/>
-      <c r="J79" s="53"/>
-      <c r="K79" s="53"/>
+      <c r="B79" s="107"/>
+      <c r="C79" s="107"/>
+      <c r="D79" s="107"/>
+      <c r="E79" s="107"/>
+      <c r="H79" s="53"/>
+      <c r="I79" s="55"/>
+      <c r="J79" s="55"/>
+      <c r="K79" s="55"/>
       <c r="L79" s="27"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B80" s="105"/>
-      <c r="C80" s="105"/>
-      <c r="D80" s="105"/>
-      <c r="E80" s="105"/>
-      <c r="H80" s="51"/>
-      <c r="I80" s="53"/>
-      <c r="J80" s="53"/>
-      <c r="K80" s="53"/>
+      <c r="B80" s="107"/>
+      <c r="C80" s="107"/>
+      <c r="D80" s="107"/>
+      <c r="E80" s="107"/>
+      <c r="H80" s="53"/>
+      <c r="I80" s="55"/>
+      <c r="J80" s="55"/>
+      <c r="K80" s="55"/>
       <c r="L80" s="27"/>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B81" s="106">
+      <c r="B81" s="108">
         <f>D9</f>
         <v>0</v>
       </c>
-      <c r="C81" s="106">
+      <c r="C81" s="108">
         <f>C74</f>
         <v>0</v>
       </c>
-      <c r="D81" s="106">
+      <c r="D81" s="108">
         <f>SALES!B205</f>
         <v>0</v>
       </c>
-      <c r="E81" s="106">
+      <c r="E81" s="108">
         <f>B81-(C81+D81)</f>
         <v>0</v>
       </c>
-      <c r="H81" s="52" t="e">
+      <c r="H81" s="54" t="e">
         <f>SALES!I205</f>
         <v>#DIV/0!</v>
       </c>
@@ -3365,22 +3387,22 @@
       <c r="L81" s="27"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B82" s="106"/>
-      <c r="C82" s="106"/>
-      <c r="D82" s="106"/>
-      <c r="E82" s="106"/>
-      <c r="H82" s="52"/>
+      <c r="B82" s="108"/>
+      <c r="C82" s="108"/>
+      <c r="D82" s="108"/>
+      <c r="E82" s="108"/>
+      <c r="H82" s="54"/>
       <c r="I82" s="27"/>
       <c r="J82" s="27"/>
       <c r="K82" s="27"/>
       <c r="L82" s="27"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B83" s="106"/>
-      <c r="C83" s="106"/>
-      <c r="D83" s="106"/>
-      <c r="E83" s="106"/>
-      <c r="H83" s="52"/>
+      <c r="B83" s="108"/>
+      <c r="C83" s="108"/>
+      <c r="D83" s="108"/>
+      <c r="E83" s="108"/>
+      <c r="H83" s="54"/>
       <c r="I83" s="27"/>
       <c r="J83" s="27"/>
       <c r="K83" s="27"/>
@@ -3405,15 +3427,15 @@
       <c r="L86" s="27"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I87" s="53"/>
-      <c r="J87" s="54"/>
-      <c r="K87" s="54"/>
+      <c r="I87" s="55"/>
+      <c r="J87" s="56"/>
+      <c r="K87" s="56"/>
       <c r="L87" s="27"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I88" s="53"/>
-      <c r="J88" s="54"/>
-      <c r="K88" s="54"/>
+      <c r="I88" s="55"/>
+      <c r="J88" s="56"/>
+      <c r="K88" s="56"/>
       <c r="L88" s="27"/>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.3">
@@ -3494,93 +3516,93 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D2" s="139" t="s">
+      <c r="D2" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="141" t="s">
+      <c r="B6" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="145"/>
-      <c r="E6" s="78" t="s">
+      <c r="D6" s="147"/>
+      <c r="E6" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="144" t="s">
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="146"/>
-      <c r="K6" s="147"/>
-      <c r="L6" s="144" t="s">
+      <c r="J6" s="148"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="146" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="145"/>
+      <c r="M6" s="147"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="142"/>
-      <c r="C7" s="148" t="s">
+      <c r="B7" s="144"/>
+      <c r="C7" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="141" t="s">
+      <c r="D7" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="141" t="s">
+      <c r="E7" s="143" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="141" t="s">
+      <c r="F7" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="141" t="s">
+      <c r="G7" s="143" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="141" t="s">
+      <c r="H7" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="150" t="s">
+      <c r="I7" s="152" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="151"/>
-      <c r="K7" s="154" t="s">
+      <c r="J7" s="153"/>
+      <c r="K7" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="137" t="s">
+      <c r="L7" s="139" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="137" t="s">
+      <c r="M7" s="139" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="143"/>
-      <c r="C8" s="149"/>
-      <c r="D8" s="143"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="152"/>
-      <c r="J8" s="153"/>
-      <c r="K8" s="155"/>
-      <c r="L8" s="138"/>
-      <c r="M8" s="138"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="155"/>
+      <c r="K8" s="157"/>
+      <c r="L8" s="140"/>
+      <c r="M8" s="140"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="48"/>
@@ -3593,8 +3615,8 @@
         <f>F9*G9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
       <c r="K9" s="41"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -3613,8 +3635,8 @@
         <f t="shared" ref="H10:H58" si="0">F10*G10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="129"/>
-      <c r="J10" s="129"/>
+      <c r="I10" s="131"/>
+      <c r="J10" s="131"/>
       <c r="K10" s="13"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -3624,10 +3646,10 @@
         <f t="shared" ref="B11:B58" si="1">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="134">
+      <c r="D11" s="136">
         <f>C9*D9</f>
         <v>0</v>
       </c>
@@ -3638,8 +3660,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="129"/>
-      <c r="J11" s="129"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="131"/>
       <c r="K11" s="13"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
@@ -3649,8 +3671,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C12" s="132"/>
-      <c r="D12" s="135"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="137"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -3658,8 +3680,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="129"/>
-      <c r="J12" s="129"/>
+      <c r="I12" s="131"/>
+      <c r="J12" s="131"/>
       <c r="K12" s="13"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -3669,8 +3691,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C13" s="132"/>
-      <c r="D13" s="135"/>
+      <c r="C13" s="134"/>
+      <c r="D13" s="137"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -3678,8 +3700,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
+      <c r="I13" s="131"/>
+      <c r="J13" s="131"/>
       <c r="K13" s="13"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -3689,8 +3711,8 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="135"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="137"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -3698,8 +3720,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="129"/>
-      <c r="J14" s="129"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="131"/>
       <c r="K14" s="13"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -3709,8 +3731,8 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C15" s="132"/>
-      <c r="D15" s="135"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="137"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -3718,8 +3740,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="129"/>
-      <c r="J15" s="129"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="131"/>
       <c r="K15" s="13"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -3729,8 +3751,8 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C16" s="133"/>
-      <c r="D16" s="136"/>
+      <c r="C16" s="135"/>
+      <c r="D16" s="138"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -3738,8 +3760,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="129"/>
-      <c r="J16" s="129"/>
+      <c r="I16" s="131"/>
+      <c r="J16" s="131"/>
       <c r="K16" s="13"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
@@ -3758,8 +3780,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="129"/>
-      <c r="J17" s="129"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="131"/>
       <c r="K17" s="13"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -3778,8 +3800,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="129"/>
-      <c r="J18" s="129"/>
+      <c r="I18" s="131"/>
+      <c r="J18" s="131"/>
       <c r="K18" s="13"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -3798,8 +3820,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="129"/>
-      <c r="J19" s="129"/>
+      <c r="I19" s="131"/>
+      <c r="J19" s="131"/>
       <c r="K19" s="13"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -3818,8 +3840,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="129"/>
-      <c r="J20" s="129"/>
+      <c r="I20" s="131"/>
+      <c r="J20" s="131"/>
       <c r="K20" s="13"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
@@ -3838,8 +3860,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="129"/>
-      <c r="J21" s="129"/>
+      <c r="I21" s="131"/>
+      <c r="J21" s="131"/>
       <c r="K21" s="13"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
@@ -3858,8 +3880,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="129"/>
-      <c r="J22" s="129"/>
+      <c r="I22" s="131"/>
+      <c r="J22" s="131"/>
       <c r="K22" s="13"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -3878,8 +3900,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="129"/>
-      <c r="J23" s="129"/>
+      <c r="I23" s="131"/>
+      <c r="J23" s="131"/>
       <c r="K23" s="13"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
@@ -3898,8 +3920,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="129"/>
-      <c r="J24" s="129"/>
+      <c r="I24" s="131"/>
+      <c r="J24" s="131"/>
       <c r="K24" s="13"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
@@ -3918,8 +3940,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="129"/>
-      <c r="J25" s="129"/>
+      <c r="I25" s="131"/>
+      <c r="J25" s="131"/>
       <c r="K25" s="13"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
@@ -3938,8 +3960,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26" s="129"/>
-      <c r="J26" s="129"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
       <c r="K26" s="13"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -3958,8 +3980,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
+      <c r="I27" s="131"/>
+      <c r="J27" s="131"/>
       <c r="K27" s="13"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
@@ -3978,8 +4000,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="129"/>
-      <c r="J28" s="129"/>
+      <c r="I28" s="131"/>
+      <c r="J28" s="131"/>
       <c r="K28" s="13"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
@@ -3998,8 +4020,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="129"/>
-      <c r="J29" s="129"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="131"/>
       <c r="K29" s="13"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
@@ -4018,8 +4040,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I30" s="129"/>
-      <c r="J30" s="129"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="131"/>
       <c r="K30" s="13"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
@@ -4038,8 +4060,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="129"/>
-      <c r="J31" s="129"/>
+      <c r="I31" s="131"/>
+      <c r="J31" s="131"/>
       <c r="K31" s="13"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
@@ -4058,8 +4080,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I32" s="129"/>
-      <c r="J32" s="129"/>
+      <c r="I32" s="131"/>
+      <c r="J32" s="131"/>
       <c r="K32" s="13"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
@@ -4078,8 +4100,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I33" s="129"/>
-      <c r="J33" s="129"/>
+      <c r="I33" s="131"/>
+      <c r="J33" s="131"/>
       <c r="K33" s="13"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
@@ -4098,8 +4120,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I34" s="129"/>
-      <c r="J34" s="129"/>
+      <c r="I34" s="131"/>
+      <c r="J34" s="131"/>
       <c r="K34" s="13"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
@@ -4118,8 +4140,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I35" s="129"/>
-      <c r="J35" s="129"/>
+      <c r="I35" s="131"/>
+      <c r="J35" s="131"/>
       <c r="K35" s="13"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
@@ -4138,8 +4160,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="129"/>
-      <c r="J36" s="129"/>
+      <c r="I36" s="131"/>
+      <c r="J36" s="131"/>
       <c r="K36" s="13"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -4158,8 +4180,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="129"/>
-      <c r="J37" s="129"/>
+      <c r="I37" s="131"/>
+      <c r="J37" s="131"/>
       <c r="K37" s="13"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
@@ -4178,8 +4200,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="129"/>
-      <c r="J38" s="129"/>
+      <c r="I38" s="131"/>
+      <c r="J38" s="131"/>
       <c r="K38" s="13"/>
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
@@ -4198,8 +4220,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="129"/>
-      <c r="J39" s="129"/>
+      <c r="I39" s="131"/>
+      <c r="J39" s="131"/>
       <c r="K39" s="13"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
@@ -4218,8 +4240,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="129"/>
-      <c r="J40" s="129"/>
+      <c r="I40" s="131"/>
+      <c r="J40" s="131"/>
       <c r="K40" s="13"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
@@ -4238,8 +4260,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="129"/>
-      <c r="J41" s="129"/>
+      <c r="I41" s="131"/>
+      <c r="J41" s="131"/>
       <c r="K41" s="13"/>
       <c r="L41" s="7"/>
       <c r="M41" s="7"/>
@@ -4258,8 +4280,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="129"/>
-      <c r="J42" s="129"/>
+      <c r="I42" s="131"/>
+      <c r="J42" s="131"/>
       <c r="K42" s="13"/>
       <c r="L42" s="7"/>
       <c r="M42" s="7"/>
@@ -4278,8 +4300,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I43" s="129"/>
-      <c r="J43" s="129"/>
+      <c r="I43" s="131"/>
+      <c r="J43" s="131"/>
       <c r="K43" s="13"/>
       <c r="L43" s="7"/>
       <c r="M43" s="7"/>
@@ -4298,8 +4320,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I44" s="129"/>
-      <c r="J44" s="129"/>
+      <c r="I44" s="131"/>
+      <c r="J44" s="131"/>
       <c r="K44" s="13"/>
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
@@ -4318,8 +4340,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I45" s="129"/>
-      <c r="J45" s="129"/>
+      <c r="I45" s="131"/>
+      <c r="J45" s="131"/>
       <c r="K45" s="13"/>
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
@@ -4338,8 +4360,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I46" s="129"/>
-      <c r="J46" s="129"/>
+      <c r="I46" s="131"/>
+      <c r="J46" s="131"/>
       <c r="K46" s="13"/>
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
@@ -4358,8 +4380,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I47" s="129"/>
-      <c r="J47" s="129"/>
+      <c r="I47" s="131"/>
+      <c r="J47" s="131"/>
       <c r="K47" s="13"/>
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
@@ -4378,8 +4400,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I48" s="129"/>
-      <c r="J48" s="129"/>
+      <c r="I48" s="131"/>
+      <c r="J48" s="131"/>
       <c r="K48" s="13"/>
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
@@ -4398,8 +4420,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I49" s="129"/>
-      <c r="J49" s="129"/>
+      <c r="I49" s="131"/>
+      <c r="J49" s="131"/>
       <c r="K49" s="13"/>
       <c r="L49" s="7"/>
       <c r="M49" s="7"/>
@@ -4418,8 +4440,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I50" s="129"/>
-      <c r="J50" s="129"/>
+      <c r="I50" s="131"/>
+      <c r="J50" s="131"/>
       <c r="K50" s="13"/>
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
@@ -4438,8 +4460,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I51" s="129"/>
-      <c r="J51" s="129"/>
+      <c r="I51" s="131"/>
+      <c r="J51" s="131"/>
       <c r="K51" s="13"/>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
@@ -4458,8 +4480,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I52" s="129"/>
-      <c r="J52" s="129"/>
+      <c r="I52" s="131"/>
+      <c r="J52" s="131"/>
       <c r="K52" s="13"/>
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
@@ -4478,8 +4500,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I53" s="129"/>
-      <c r="J53" s="129"/>
+      <c r="I53" s="131"/>
+      <c r="J53" s="131"/>
       <c r="K53" s="13"/>
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
@@ -4498,8 +4520,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I54" s="129"/>
-      <c r="J54" s="129"/>
+      <c r="I54" s="131"/>
+      <c r="J54" s="131"/>
       <c r="K54" s="13"/>
       <c r="L54" s="7"/>
       <c r="M54" s="7"/>
@@ -4518,8 +4540,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I55" s="129"/>
-      <c r="J55" s="129"/>
+      <c r="I55" s="131"/>
+      <c r="J55" s="131"/>
       <c r="K55" s="13"/>
       <c r="L55" s="7"/>
       <c r="M55" s="7"/>
@@ -4538,8 +4560,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I56" s="129"/>
-      <c r="J56" s="129"/>
+      <c r="I56" s="131"/>
+      <c r="J56" s="131"/>
       <c r="K56" s="13"/>
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
@@ -4558,8 +4580,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I57" s="129"/>
-      <c r="J57" s="129"/>
+      <c r="I57" s="131"/>
+      <c r="J57" s="131"/>
       <c r="K57" s="13"/>
       <c r="L57" s="12"/>
       <c r="M57" s="7"/>
@@ -4578,10 +4600,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I58" s="128" t="s">
+      <c r="I58" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="J58" s="128"/>
+      <c r="J58" s="130"/>
       <c r="K58" s="12">
         <f>SALES!L205</f>
         <v>0</v>
@@ -4620,29 +4642,29 @@
     </row>
     <row r="65" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="66" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D66" s="116" t="s">
+      <c r="D66" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="117"/>
-      <c r="F66" s="118"/>
-      <c r="G66" s="98">
+      <c r="E66" s="119"/>
+      <c r="F66" s="120"/>
+      <c r="G66" s="100">
         <f>D11</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D67" s="119"/>
-      <c r="E67" s="120"/>
-      <c r="F67" s="121"/>
-      <c r="G67" s="90"/>
+      <c r="D67" s="121"/>
+      <c r="E67" s="122"/>
+      <c r="F67" s="123"/>
+      <c r="G67" s="92"/>
     </row>
     <row r="68" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D68" s="122" t="s">
+      <c r="D68" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="123"/>
-      <c r="F68" s="124"/>
-      <c r="G68" s="98">
+      <c r="E68" s="125"/>
+      <c r="F68" s="126"/>
+      <c r="G68" s="100">
         <f>F59</f>
         <v>0</v>
       </c>
@@ -4654,10 +4676,10 @@
       <c r="O68" s="27"/>
     </row>
     <row r="69" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D69" s="125"/>
-      <c r="E69" s="126"/>
-      <c r="F69" s="127"/>
-      <c r="G69" s="90"/>
+      <c r="D69" s="127"/>
+      <c r="E69" s="128"/>
+      <c r="F69" s="129"/>
+      <c r="G69" s="92"/>
       <c r="J69" s="27"/>
       <c r="K69" s="27"/>
       <c r="L69" s="27"/>
@@ -4666,167 +4688,167 @@
       <c r="O69" s="27"/>
     </row>
     <row r="70" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D70" s="122" t="s">
+      <c r="D70" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="E70" s="123"/>
-      <c r="F70" s="124"/>
-      <c r="G70" s="98">
+      <c r="E70" s="125"/>
+      <c r="F70" s="126"/>
+      <c r="G70" s="100">
         <f>H59</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="4:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D71" s="125"/>
-      <c r="E71" s="126"/>
-      <c r="F71" s="127"/>
-      <c r="G71" s="90"/>
-      <c r="O71" s="51" t="s">
+      <c r="D71" s="127"/>
+      <c r="E71" s="128"/>
+      <c r="F71" s="129"/>
+      <c r="G71" s="92"/>
+      <c r="O71" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="72" spans="4:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="116" t="s">
+      <c r="D72" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E72" s="117"/>
-      <c r="F72" s="118"/>
-      <c r="G72" s="98">
+      <c r="E72" s="119"/>
+      <c r="F72" s="120"/>
+      <c r="G72" s="100">
         <f>K59</f>
         <v>0</v>
       </c>
-      <c r="K72" s="52" t="s">
+      <c r="K72" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="L72" s="52" t="s">
+      <c r="L72" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="M72" s="52" t="s">
+      <c r="M72" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="N72" s="109" t="s">
+      <c r="N72" s="111" t="s">
         <v>62</v>
       </c>
-      <c r="O72" s="52"/>
+      <c r="O72" s="54"/>
     </row>
     <row r="73" spans="4:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D73" s="119"/>
-      <c r="E73" s="120"/>
-      <c r="F73" s="121"/>
-      <c r="G73" s="90"/>
-      <c r="K73" s="52"/>
-      <c r="L73" s="52"/>
-      <c r="M73" s="52"/>
-      <c r="N73" s="109"/>
-      <c r="O73" s="52"/>
+      <c r="D73" s="121"/>
+      <c r="E73" s="122"/>
+      <c r="F73" s="123"/>
+      <c r="G73" s="92"/>
+      <c r="K73" s="54"/>
+      <c r="L73" s="54"/>
+      <c r="M73" s="54"/>
+      <c r="N73" s="111"/>
+      <c r="O73" s="54"/>
     </row>
     <row r="74" spans="4:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D74" s="116" t="s">
+      <c r="D74" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E74" s="117"/>
-      <c r="F74" s="118"/>
-      <c r="G74" s="98">
+      <c r="E74" s="119"/>
+      <c r="F74" s="120"/>
+      <c r="G74" s="100">
         <f>M59</f>
         <v>0</v>
       </c>
-      <c r="K74" s="52">
+      <c r="K74" s="54">
         <f>SALES!B205</f>
         <v>0</v>
       </c>
-      <c r="L74" s="52">
+      <c r="L74" s="54">
         <f>SALES!C205</f>
         <v>0</v>
       </c>
-      <c r="M74" s="52">
+      <c r="M74" s="54">
         <f>SALES!D205</f>
         <v>0</v>
       </c>
-      <c r="N74" s="109">
+      <c r="N74" s="111">
         <f>SALES!E205</f>
         <v>0</v>
       </c>
-      <c r="O74" s="52">
+      <c r="O74" s="54">
         <f>SALES!F205</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D75" s="119"/>
-      <c r="E75" s="120"/>
-      <c r="F75" s="121"/>
-      <c r="G75" s="90"/>
-      <c r="K75" s="52"/>
-      <c r="L75" s="52"/>
-      <c r="M75" s="52"/>
-      <c r="N75" s="109"/>
-      <c r="O75" s="52"/>
+      <c r="D75" s="121"/>
+      <c r="E75" s="122"/>
+      <c r="F75" s="123"/>
+      <c r="G75" s="92"/>
+      <c r="K75" s="54"/>
+      <c r="L75" s="54"/>
+      <c r="M75" s="54"/>
+      <c r="N75" s="111"/>
+      <c r="O75" s="54"/>
     </row>
     <row r="76" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D76" s="116" t="s">
+      <c r="D76" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="E76" s="117"/>
-      <c r="F76" s="118"/>
-      <c r="G76" s="98"/>
-      <c r="K76" s="52"/>
-      <c r="L76" s="52"/>
-      <c r="M76" s="52"/>
-      <c r="N76" s="109"/>
-      <c r="O76" s="52"/>
+      <c r="E76" s="119"/>
+      <c r="F76" s="120"/>
+      <c r="G76" s="100"/>
+      <c r="K76" s="54"/>
+      <c r="L76" s="54"/>
+      <c r="M76" s="54"/>
+      <c r="N76" s="111"/>
+      <c r="O76" s="54"/>
     </row>
     <row r="77" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D77" s="119"/>
-      <c r="E77" s="120"/>
-      <c r="F77" s="121"/>
-      <c r="G77" s="90"/>
+      <c r="D77" s="121"/>
+      <c r="E77" s="122"/>
+      <c r="F77" s="123"/>
+      <c r="G77" s="92"/>
     </row>
     <row r="78" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D78" s="110" t="s">
+      <c r="D78" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="E78" s="111"/>
-      <c r="F78" s="112"/>
-      <c r="G78" s="98">
+      <c r="E78" s="113"/>
+      <c r="F78" s="114"/>
+      <c r="G78" s="100">
         <f>G66+G70+G72+G74+G76</f>
         <v>0</v>
       </c>
-      <c r="K78" s="108" t="s">
+      <c r="K78" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="L78" s="108" t="s">
+      <c r="L78" s="110" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="4:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D79" s="113"/>
-      <c r="E79" s="114"/>
-      <c r="F79" s="115"/>
-      <c r="G79" s="90"/>
-      <c r="K79" s="108"/>
-      <c r="L79" s="108"/>
+      <c r="D79" s="115"/>
+      <c r="E79" s="116"/>
+      <c r="F79" s="117"/>
+      <c r="G79" s="92"/>
+      <c r="K79" s="110"/>
+      <c r="L79" s="110"/>
     </row>
     <row r="80" spans="4:15" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K80" s="108"/>
-      <c r="L80" s="108"/>
+      <c r="K80" s="110"/>
+      <c r="L80" s="110"/>
     </row>
     <row r="81" spans="11:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K81" s="107">
+      <c r="K81" s="109">
         <f>SALES!H205</f>
         <v>0</v>
       </c>
-      <c r="L81" s="106" t="e">
+      <c r="L81" s="108" t="e">
         <f>SALES!I205</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="82" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K82" s="106"/>
-      <c r="L82" s="106"/>
+      <c r="K82" s="108"/>
+      <c r="L82" s="108"/>
     </row>
     <row r="83" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K83" s="106"/>
-      <c r="L83" s="106"/>
+      <c r="K83" s="108"/>
+      <c r="L83" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="96">
@@ -4935,8 +4957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06126A5B-91A0-41E1-A06A-A0919D230834}">
   <dimension ref="B3:P494"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F446" sqref="F446:G447"/>
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4946,13 +4968,13 @@
       <c r="B4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="175"/>
-      <c r="D4" s="176"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="178"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="177"/>
-      <c r="H4" s="178"/>
+      <c r="G4" s="179"/>
+      <c r="H4" s="180"/>
       <c r="J4" s="11" t="s">
         <v>39</v>
       </c>
@@ -4960,15 +4982,15 @@
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="F6" s="156" t="s">
+      <c r="D6" s="85"/>
+      <c r="F6" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="179"/>
-      <c r="H6" s="157"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="159"/>
       <c r="J6" s="11" t="s">
         <v>42</v>
       </c>
@@ -5008,10 +5030,10 @@
       </c>
       <c r="J8" s="37"/>
       <c r="K8" s="7"/>
-      <c r="O8" s="182" t="s">
+      <c r="O8" s="184" t="s">
         <v>70</v>
       </c>
-      <c r="P8" s="183">
+      <c r="P8" s="185">
         <v>4</v>
       </c>
     </row>
@@ -5026,8 +5048,8 @@
       </c>
       <c r="J9" s="37"/>
       <c r="K9" s="7"/>
-      <c r="O9" s="182"/>
-      <c r="P9" s="183"/>
+      <c r="O9" s="184"/>
+      <c r="P9" s="185"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C10" s="7"/>
@@ -5040,8 +5062,8 @@
       </c>
       <c r="J10" s="37"/>
       <c r="K10" s="7"/>
-      <c r="O10" s="182"/>
-      <c r="P10" s="183"/>
+      <c r="O10" s="184"/>
+      <c r="P10" s="185"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C11" s="7"/>
@@ -5054,8 +5076,8 @@
       </c>
       <c r="J11" s="37"/>
       <c r="K11" s="7"/>
-      <c r="O11" s="182"/>
-      <c r="P11" s="183"/>
+      <c r="O11" s="184"/>
+      <c r="P11" s="185"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C12" s="7"/>
@@ -5226,85 +5248,85 @@
     </row>
     <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H26" s="156" t="s">
+      <c r="H26" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I26" s="160"/>
-      <c r="J26" s="163">
+      <c r="I26" s="162"/>
+      <c r="J26" s="165">
         <f>J23-D23</f>
         <v>0</v>
       </c>
-      <c r="K26" s="164"/>
+      <c r="K26" s="166"/>
     </row>
     <row r="27" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H27" s="161"/>
-      <c r="I27" s="162"/>
-      <c r="J27" s="165"/>
-      <c r="K27" s="166"/>
+      <c r="H27" s="163"/>
+      <c r="I27" s="164"/>
+      <c r="J27" s="167"/>
+      <c r="K27" s="168"/>
     </row>
     <row r="29" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D30" s="156" t="s">
+      <c r="D30" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="157"/>
-      <c r="F30" s="167"/>
-      <c r="G30" s="168"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="169"/>
+      <c r="G30" s="170"/>
     </row>
     <row r="31" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="158"/>
-      <c r="E31" s="159"/>
-      <c r="F31" s="169"/>
-      <c r="G31" s="170"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="161"/>
+      <c r="F31" s="171"/>
+      <c r="G31" s="172"/>
     </row>
     <row r="32" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D33" s="156" t="s">
+      <c r="D33" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="157"/>
-      <c r="F33" s="171">
+      <c r="E33" s="159"/>
+      <c r="F33" s="173">
         <f>J26*F30</f>
         <v>0</v>
       </c>
-      <c r="G33" s="172"/>
+      <c r="G33" s="174"/>
     </row>
     <row r="34" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="158"/>
-      <c r="E34" s="159"/>
-      <c r="F34" s="173"/>
-      <c r="G34" s="174"/>
+      <c r="D34" s="160"/>
+      <c r="E34" s="161"/>
+      <c r="F34" s="175"/>
+      <c r="G34" s="176"/>
     </row>
     <row r="35" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D36" s="156" t="s">
+      <c r="D36" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="157"/>
-      <c r="F36" s="156" t="e">
+      <c r="E36" s="159"/>
+      <c r="F36" s="158" t="e">
         <f>J26/H23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G36" s="157"/>
+      <c r="G36" s="159"/>
     </row>
     <row r="37" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D37" s="158"/>
-      <c r="E37" s="159"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="159"/>
+      <c r="D37" s="160"/>
+      <c r="E37" s="161"/>
+      <c r="F37" s="160"/>
+      <c r="G37" s="161"/>
     </row>
     <row r="42" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="175"/>
-      <c r="D43" s="176"/>
+      <c r="C43" s="177"/>
+      <c r="D43" s="178"/>
       <c r="F43" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="177"/>
-      <c r="H43" s="178"/>
+      <c r="G43" s="179"/>
+      <c r="H43" s="180"/>
       <c r="J43" s="11" t="s">
         <v>39</v>
       </c>
@@ -5312,15 +5334,15 @@
     </row>
     <row r="44" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="78" t="s">
+      <c r="C45" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="83"/>
-      <c r="F45" s="156" t="s">
+      <c r="D45" s="85"/>
+      <c r="F45" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G45" s="179"/>
-      <c r="H45" s="157"/>
+      <c r="G45" s="181"/>
+      <c r="H45" s="159"/>
       <c r="J45" s="11" t="s">
         <v>42</v>
       </c>
@@ -5566,85 +5588,85 @@
     </row>
     <row r="64" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="65" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="H65" s="156" t="s">
+      <c r="H65" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I65" s="160"/>
-      <c r="J65" s="163">
+      <c r="I65" s="162"/>
+      <c r="J65" s="165">
         <f>J62-D62</f>
         <v>0</v>
       </c>
-      <c r="K65" s="164"/>
+      <c r="K65" s="166"/>
     </row>
     <row r="66" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H66" s="161"/>
-      <c r="I66" s="162"/>
-      <c r="J66" s="165"/>
-      <c r="K66" s="166"/>
+      <c r="H66" s="163"/>
+      <c r="I66" s="164"/>
+      <c r="J66" s="167"/>
+      <c r="K66" s="168"/>
     </row>
     <row r="68" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="69" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D69" s="156" t="s">
+      <c r="D69" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E69" s="157"/>
-      <c r="F69" s="167"/>
-      <c r="G69" s="168"/>
+      <c r="E69" s="159"/>
+      <c r="F69" s="169"/>
+      <c r="G69" s="170"/>
     </row>
     <row r="70" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D70" s="158"/>
-      <c r="E70" s="159"/>
-      <c r="F70" s="169"/>
-      <c r="G70" s="170"/>
+      <c r="D70" s="160"/>
+      <c r="E70" s="161"/>
+      <c r="F70" s="171"/>
+      <c r="G70" s="172"/>
     </row>
     <row r="71" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D72" s="156" t="s">
+      <c r="D72" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E72" s="157"/>
-      <c r="F72" s="171">
+      <c r="E72" s="159"/>
+      <c r="F72" s="173">
         <f>J65*F69</f>
         <v>0</v>
       </c>
-      <c r="G72" s="172"/>
+      <c r="G72" s="174"/>
     </row>
     <row r="73" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D73" s="158"/>
-      <c r="E73" s="159"/>
-      <c r="F73" s="173"/>
-      <c r="G73" s="174"/>
+      <c r="D73" s="160"/>
+      <c r="E73" s="161"/>
+      <c r="F73" s="175"/>
+      <c r="G73" s="176"/>
     </row>
     <row r="74" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="75" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D75" s="156" t="s">
+      <c r="D75" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E75" s="157"/>
-      <c r="F75" s="156" t="e">
+      <c r="E75" s="159"/>
+      <c r="F75" s="158" t="e">
         <f>J65/H62</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G75" s="157"/>
+      <c r="G75" s="159"/>
     </row>
     <row r="76" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D76" s="158"/>
-      <c r="E76" s="159"/>
-      <c r="F76" s="158"/>
-      <c r="G76" s="159"/>
+      <c r="D76" s="160"/>
+      <c r="E76" s="161"/>
+      <c r="F76" s="160"/>
+      <c r="G76" s="161"/>
     </row>
     <row r="82" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="83" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B83" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C83" s="175"/>
-      <c r="D83" s="176"/>
+      <c r="C83" s="177"/>
+      <c r="D83" s="178"/>
       <c r="F83" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G83" s="177"/>
-      <c r="H83" s="178"/>
+      <c r="G83" s="179"/>
+      <c r="H83" s="180"/>
       <c r="J83" s="11" t="s">
         <v>39</v>
       </c>
@@ -5652,15 +5674,15 @@
     </row>
     <row r="84" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="85" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C85" s="78" t="s">
+      <c r="C85" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D85" s="83"/>
-      <c r="F85" s="156" t="s">
+      <c r="D85" s="85"/>
+      <c r="F85" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G85" s="179"/>
-      <c r="H85" s="157"/>
+      <c r="G85" s="181"/>
+      <c r="H85" s="159"/>
       <c r="J85" s="11" t="s">
         <v>42</v>
       </c>
@@ -5906,85 +5928,85 @@
     </row>
     <row r="104" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="105" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H105" s="156" t="s">
+      <c r="H105" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I105" s="160"/>
-      <c r="J105" s="163">
+      <c r="I105" s="162"/>
+      <c r="J105" s="165">
         <f>J102-D102</f>
         <v>0</v>
       </c>
-      <c r="K105" s="164"/>
+      <c r="K105" s="166"/>
     </row>
     <row r="106" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H106" s="161"/>
-      <c r="I106" s="162"/>
-      <c r="J106" s="165"/>
-      <c r="K106" s="166"/>
+      <c r="H106" s="163"/>
+      <c r="I106" s="164"/>
+      <c r="J106" s="167"/>
+      <c r="K106" s="168"/>
     </row>
     <row r="108" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="109" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D109" s="156" t="s">
+      <c r="D109" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E109" s="157"/>
-      <c r="F109" s="167"/>
-      <c r="G109" s="168"/>
+      <c r="E109" s="159"/>
+      <c r="F109" s="169"/>
+      <c r="G109" s="170"/>
     </row>
     <row r="110" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D110" s="158"/>
-      <c r="E110" s="159"/>
-      <c r="F110" s="169"/>
-      <c r="G110" s="170"/>
+      <c r="D110" s="160"/>
+      <c r="E110" s="161"/>
+      <c r="F110" s="171"/>
+      <c r="G110" s="172"/>
     </row>
     <row r="111" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="112" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D112" s="156" t="s">
+      <c r="D112" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E112" s="157"/>
-      <c r="F112" s="171">
+      <c r="E112" s="159"/>
+      <c r="F112" s="173">
         <f>J105*F109</f>
         <v>0</v>
       </c>
-      <c r="G112" s="172"/>
+      <c r="G112" s="174"/>
     </row>
     <row r="113" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D113" s="158"/>
-      <c r="E113" s="159"/>
-      <c r="F113" s="173"/>
-      <c r="G113" s="174"/>
+      <c r="D113" s="160"/>
+      <c r="E113" s="161"/>
+      <c r="F113" s="175"/>
+      <c r="G113" s="176"/>
     </row>
     <row r="114" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="115" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D115" s="156" t="s">
+      <c r="D115" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E115" s="157"/>
-      <c r="F115" s="156" t="e">
+      <c r="E115" s="159"/>
+      <c r="F115" s="158" t="e">
         <f>J105/H102</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G115" s="157"/>
+      <c r="G115" s="159"/>
     </row>
     <row r="116" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D116" s="158"/>
-      <c r="E116" s="159"/>
-      <c r="F116" s="158"/>
-      <c r="G116" s="159"/>
+      <c r="D116" s="160"/>
+      <c r="E116" s="161"/>
+      <c r="F116" s="160"/>
+      <c r="G116" s="161"/>
     </row>
     <row r="121" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="122" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B122" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C122" s="175"/>
-      <c r="D122" s="176"/>
+      <c r="C122" s="177"/>
+      <c r="D122" s="178"/>
       <c r="F122" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G122" s="177"/>
-      <c r="H122" s="178"/>
+      <c r="G122" s="179"/>
+      <c r="H122" s="180"/>
       <c r="J122" s="11" t="s">
         <v>39</v>
       </c>
@@ -5992,15 +6014,15 @@
     </row>
     <row r="123" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="124" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C124" s="78" t="s">
+      <c r="C124" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D124" s="83"/>
-      <c r="F124" s="156" t="s">
+      <c r="D124" s="85"/>
+      <c r="F124" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G124" s="179"/>
-      <c r="H124" s="157"/>
+      <c r="G124" s="181"/>
+      <c r="H124" s="159"/>
       <c r="J124" s="11" t="s">
         <v>42</v>
       </c>
@@ -6246,85 +6268,85 @@
     </row>
     <row r="143" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="144" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H144" s="156" t="s">
+      <c r="H144" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I144" s="160"/>
-      <c r="J144" s="163">
+      <c r="I144" s="162"/>
+      <c r="J144" s="165">
         <f>J141-D141</f>
         <v>0</v>
       </c>
-      <c r="K144" s="164"/>
+      <c r="K144" s="166"/>
     </row>
     <row r="145" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H145" s="161"/>
-      <c r="I145" s="162"/>
-      <c r="J145" s="165"/>
-      <c r="K145" s="166"/>
+      <c r="H145" s="163"/>
+      <c r="I145" s="164"/>
+      <c r="J145" s="167"/>
+      <c r="K145" s="168"/>
     </row>
     <row r="147" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="148" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D148" s="156" t="s">
+      <c r="D148" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E148" s="157"/>
-      <c r="F148" s="167"/>
-      <c r="G148" s="168"/>
+      <c r="E148" s="159"/>
+      <c r="F148" s="169"/>
+      <c r="G148" s="170"/>
     </row>
     <row r="149" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D149" s="158"/>
-      <c r="E149" s="159"/>
-      <c r="F149" s="169"/>
-      <c r="G149" s="170"/>
+      <c r="D149" s="160"/>
+      <c r="E149" s="161"/>
+      <c r="F149" s="171"/>
+      <c r="G149" s="172"/>
     </row>
     <row r="150" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="151" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D151" s="156" t="s">
+      <c r="D151" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E151" s="157"/>
-      <c r="F151" s="171">
+      <c r="E151" s="159"/>
+      <c r="F151" s="173">
         <f>J144*F148</f>
         <v>0</v>
       </c>
-      <c r="G151" s="172"/>
+      <c r="G151" s="174"/>
     </row>
     <row r="152" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D152" s="158"/>
-      <c r="E152" s="159"/>
-      <c r="F152" s="173"/>
-      <c r="G152" s="174"/>
+      <c r="D152" s="160"/>
+      <c r="E152" s="161"/>
+      <c r="F152" s="175"/>
+      <c r="G152" s="176"/>
     </row>
     <row r="153" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="154" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D154" s="156" t="s">
+      <c r="D154" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E154" s="157"/>
-      <c r="F154" s="156" t="e">
+      <c r="E154" s="159"/>
+      <c r="F154" s="158" t="e">
         <f>J144/H141</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G154" s="157"/>
+      <c r="G154" s="159"/>
     </row>
     <row r="155" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D155" s="158"/>
-      <c r="E155" s="159"/>
-      <c r="F155" s="158"/>
-      <c r="G155" s="159"/>
+      <c r="D155" s="160"/>
+      <c r="E155" s="161"/>
+      <c r="F155" s="160"/>
+      <c r="G155" s="161"/>
     </row>
     <row r="162" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="163" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C163" s="175"/>
-      <c r="D163" s="176"/>
+      <c r="C163" s="177"/>
+      <c r="D163" s="178"/>
       <c r="F163" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G163" s="177"/>
-      <c r="H163" s="178"/>
+      <c r="G163" s="179"/>
+      <c r="H163" s="180"/>
       <c r="J163" s="11" t="s">
         <v>39</v>
       </c>
@@ -6332,15 +6354,15 @@
     </row>
     <row r="164" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="165" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C165" s="78" t="s">
+      <c r="C165" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D165" s="83"/>
-      <c r="F165" s="156" t="s">
+      <c r="D165" s="85"/>
+      <c r="F165" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G165" s="179"/>
-      <c r="H165" s="157"/>
+      <c r="G165" s="181"/>
+      <c r="H165" s="159"/>
       <c r="J165" s="11" t="s">
         <v>42</v>
       </c>
@@ -6586,191 +6608,191 @@
     </row>
     <row r="184" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="185" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H185" s="156" t="s">
+      <c r="H185" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I185" s="160"/>
-      <c r="J185" s="163">
+      <c r="I185" s="162"/>
+      <c r="J185" s="165">
         <f>J182-D182</f>
         <v>0</v>
       </c>
-      <c r="K185" s="164"/>
+      <c r="K185" s="166"/>
     </row>
     <row r="186" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H186" s="161"/>
-      <c r="I186" s="162"/>
-      <c r="J186" s="165"/>
-      <c r="K186" s="166"/>
+      <c r="H186" s="163"/>
+      <c r="I186" s="164"/>
+      <c r="J186" s="167"/>
+      <c r="K186" s="168"/>
     </row>
     <row r="188" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="189" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D189" s="156" t="s">
+      <c r="D189" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E189" s="157"/>
-      <c r="F189" s="167"/>
-      <c r="G189" s="168"/>
+      <c r="E189" s="159"/>
+      <c r="F189" s="169"/>
+      <c r="G189" s="170"/>
     </row>
     <row r="190" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D190" s="158"/>
-      <c r="E190" s="159"/>
-      <c r="F190" s="169"/>
-      <c r="G190" s="170"/>
+      <c r="D190" s="160"/>
+      <c r="E190" s="161"/>
+      <c r="F190" s="171"/>
+      <c r="G190" s="172"/>
     </row>
     <row r="191" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="192" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D192" s="156" t="s">
+      <c r="D192" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E192" s="157"/>
-      <c r="F192" s="171">
+      <c r="E192" s="159"/>
+      <c r="F192" s="173">
         <f>J185*F189</f>
         <v>0</v>
       </c>
-      <c r="G192" s="172"/>
+      <c r="G192" s="174"/>
     </row>
     <row r="193" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D193" s="158"/>
-      <c r="E193" s="159"/>
-      <c r="F193" s="173"/>
-      <c r="G193" s="174"/>
+      <c r="D193" s="160"/>
+      <c r="E193" s="161"/>
+      <c r="F193" s="175"/>
+      <c r="G193" s="176"/>
     </row>
     <row r="194" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="195" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D195" s="156" t="s">
+      <c r="D195" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E195" s="157"/>
-      <c r="F195" s="156" t="e">
+      <c r="E195" s="159"/>
+      <c r="F195" s="158" t="e">
         <f>J185/H182</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G195" s="157"/>
+      <c r="G195" s="159"/>
     </row>
     <row r="196" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D196" s="158"/>
-      <c r="E196" s="159"/>
-      <c r="F196" s="158"/>
-      <c r="G196" s="159"/>
+      <c r="D196" s="160"/>
+      <c r="E196" s="161"/>
+      <c r="F196" s="160"/>
+      <c r="G196" s="161"/>
     </row>
     <row r="202" spans="2:12" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H202" s="105" t="s">
+      <c r="H202" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="I202" s="108" t="s">
+      <c r="I202" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="K202" s="180" t="s">
+      <c r="K202" s="182" t="s">
         <v>72</v>
       </c>
-      <c r="L202" s="180" t="s">
+      <c r="L202" s="182" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="203" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="51" t="s">
+      <c r="B203" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C203" s="51" t="s">
+      <c r="C203" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="D203" s="51" t="s">
+      <c r="D203" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="E203" s="51" t="s">
+      <c r="E203" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="F203" s="51" t="s">
+      <c r="F203" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="H203" s="105"/>
-      <c r="I203" s="108"/>
-      <c r="K203" s="180"/>
-      <c r="L203" s="180"/>
+      <c r="H203" s="107"/>
+      <c r="I203" s="110"/>
+      <c r="K203" s="182"/>
+      <c r="L203" s="182"/>
     </row>
     <row r="204" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B204" s="51"/>
-      <c r="C204" s="51"/>
-      <c r="D204" s="51"/>
-      <c r="E204" s="51"/>
-      <c r="F204" s="51"/>
-      <c r="H204" s="105"/>
-      <c r="I204" s="108"/>
-      <c r="K204" s="180"/>
-      <c r="L204" s="180"/>
+      <c r="B204" s="53"/>
+      <c r="C204" s="53"/>
+      <c r="D204" s="53"/>
+      <c r="E204" s="53"/>
+      <c r="F204" s="53"/>
+      <c r="H204" s="107"/>
+      <c r="I204" s="110"/>
+      <c r="K204" s="182"/>
+      <c r="L204" s="182"/>
     </row>
     <row r="205" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B205" s="51">
+      <c r="B205" s="53">
         <f>H23+H62+H102+H141+H182+H234+H275+H316+H357+H398+H439+H480</f>
         <v>0</v>
       </c>
-      <c r="C205" s="51">
+      <c r="C205" s="53">
         <f>[1]CHICKS!J20-[1]SALES!B205</f>
         <v>0</v>
       </c>
-      <c r="D205" s="51">
+      <c r="D205" s="53">
         <f>F33+F72+F112+F151+F192+F244+F285+F326+F367+F408+F449+F490</f>
         <v>0</v>
       </c>
-      <c r="E205" s="51">
+      <c r="E205" s="53">
         <f>[1]SALES!D205-[1]EXPENSE!G78</f>
         <v>0</v>
       </c>
-      <c r="F205" s="51">
+      <c r="F205" s="53">
         <f>D205-L205</f>
         <v>0</v>
       </c>
-      <c r="H205" s="107">
+      <c r="H205" s="109">
         <f>J185+J144+J105+J65+J26+J237+J278+J319+J360+J401+J442+J483</f>
         <v>0</v>
       </c>
-      <c r="I205" s="106" t="e">
+      <c r="I205" s="108" t="e">
         <f>H205/B205</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K205" s="181">
+      <c r="K205" s="183">
         <f>K23+K62+K102+K141+K182+K234+K275+K316+K357+K398+K439+K480</f>
         <v>0</v>
       </c>
-      <c r="L205" s="181">
+      <c r="L205" s="183">
         <f>P8*K205</f>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B206" s="51"/>
-      <c r="C206" s="51"/>
-      <c r="D206" s="51"/>
-      <c r="E206" s="51"/>
-      <c r="F206" s="51"/>
-      <c r="H206" s="106"/>
-      <c r="I206" s="106"/>
-      <c r="K206" s="181"/>
-      <c r="L206" s="181"/>
+      <c r="B206" s="53"/>
+      <c r="C206" s="53"/>
+      <c r="D206" s="53"/>
+      <c r="E206" s="53"/>
+      <c r="F206" s="53"/>
+      <c r="H206" s="108"/>
+      <c r="I206" s="108"/>
+      <c r="K206" s="183"/>
+      <c r="L206" s="183"/>
     </row>
     <row r="207" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B207" s="51"/>
-      <c r="C207" s="51"/>
-      <c r="D207" s="51"/>
-      <c r="E207" s="51"/>
-      <c r="F207" s="51"/>
-      <c r="H207" s="106"/>
-      <c r="I207" s="106"/>
-      <c r="K207" s="181"/>
-      <c r="L207" s="181"/>
+      <c r="B207" s="53"/>
+      <c r="C207" s="53"/>
+      <c r="D207" s="53"/>
+      <c r="E207" s="53"/>
+      <c r="F207" s="53"/>
+      <c r="H207" s="108"/>
+      <c r="I207" s="108"/>
+      <c r="K207" s="183"/>
+      <c r="L207" s="183"/>
     </row>
     <row r="214" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="215" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B215" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C215" s="175"/>
-      <c r="D215" s="176"/>
+      <c r="C215" s="177"/>
+      <c r="D215" s="178"/>
       <c r="F215" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G215" s="177"/>
-      <c r="H215" s="178"/>
+      <c r="G215" s="179"/>
+      <c r="H215" s="180"/>
       <c r="J215" s="11" t="s">
         <v>39</v>
       </c>
@@ -6778,15 +6800,15 @@
     </row>
     <row r="216" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="217" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C217" s="78" t="s">
+      <c r="C217" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D217" s="83"/>
-      <c r="F217" s="156" t="s">
+      <c r="D217" s="85"/>
+      <c r="F217" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G217" s="179"/>
-      <c r="H217" s="157"/>
+      <c r="G217" s="181"/>
+      <c r="H217" s="159"/>
       <c r="J217" s="11" t="s">
         <v>42</v>
       </c>
@@ -7032,85 +7054,85 @@
     </row>
     <row r="236" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="237" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H237" s="156" t="s">
+      <c r="H237" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I237" s="160"/>
-      <c r="J237" s="163">
+      <c r="I237" s="162"/>
+      <c r="J237" s="165">
         <f>J234-D234</f>
         <v>0</v>
       </c>
-      <c r="K237" s="164"/>
+      <c r="K237" s="166"/>
     </row>
     <row r="238" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H238" s="161"/>
-      <c r="I238" s="162"/>
-      <c r="J238" s="165"/>
-      <c r="K238" s="166"/>
+      <c r="H238" s="163"/>
+      <c r="I238" s="164"/>
+      <c r="J238" s="167"/>
+      <c r="K238" s="168"/>
     </row>
     <row r="240" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="241" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D241" s="156" t="s">
+      <c r="D241" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E241" s="157"/>
-      <c r="F241" s="167"/>
-      <c r="G241" s="168"/>
+      <c r="E241" s="159"/>
+      <c r="F241" s="169"/>
+      <c r="G241" s="170"/>
     </row>
     <row r="242" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D242" s="158"/>
-      <c r="E242" s="159"/>
-      <c r="F242" s="169"/>
-      <c r="G242" s="170"/>
+      <c r="D242" s="160"/>
+      <c r="E242" s="161"/>
+      <c r="F242" s="171"/>
+      <c r="G242" s="172"/>
     </row>
     <row r="243" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="244" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D244" s="156" t="s">
+      <c r="D244" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E244" s="157"/>
-      <c r="F244" s="171">
+      <c r="E244" s="159"/>
+      <c r="F244" s="173">
         <f>J237*F241</f>
         <v>0</v>
       </c>
-      <c r="G244" s="172"/>
+      <c r="G244" s="174"/>
     </row>
     <row r="245" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D245" s="158"/>
-      <c r="E245" s="159"/>
-      <c r="F245" s="173"/>
-      <c r="G245" s="174"/>
+      <c r="D245" s="160"/>
+      <c r="E245" s="161"/>
+      <c r="F245" s="175"/>
+      <c r="G245" s="176"/>
     </row>
     <row r="246" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="247" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D247" s="156" t="s">
+      <c r="D247" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E247" s="157"/>
-      <c r="F247" s="156" t="e">
+      <c r="E247" s="159"/>
+      <c r="F247" s="158" t="e">
         <f>J237/H234</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G247" s="157"/>
+      <c r="G247" s="159"/>
     </row>
     <row r="248" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D248" s="158"/>
-      <c r="E248" s="159"/>
-      <c r="F248" s="158"/>
-      <c r="G248" s="159"/>
+      <c r="D248" s="160"/>
+      <c r="E248" s="161"/>
+      <c r="F248" s="160"/>
+      <c r="G248" s="161"/>
     </row>
     <row r="255" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="256" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B256" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C256" s="175"/>
-      <c r="D256" s="176"/>
+      <c r="C256" s="177"/>
+      <c r="D256" s="178"/>
       <c r="F256" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G256" s="177"/>
-      <c r="H256" s="178"/>
+      <c r="G256" s="179"/>
+      <c r="H256" s="180"/>
       <c r="J256" s="11" t="s">
         <v>39</v>
       </c>
@@ -7118,15 +7140,15 @@
     </row>
     <row r="257" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="258" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C258" s="78" t="s">
+      <c r="C258" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D258" s="83"/>
-      <c r="F258" s="156" t="s">
+      <c r="D258" s="85"/>
+      <c r="F258" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G258" s="179"/>
-      <c r="H258" s="157"/>
+      <c r="G258" s="181"/>
+      <c r="H258" s="159"/>
       <c r="J258" s="11" t="s">
         <v>42</v>
       </c>
@@ -7372,85 +7394,85 @@
     </row>
     <row r="277" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="278" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H278" s="156" t="s">
+      <c r="H278" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I278" s="160"/>
-      <c r="J278" s="163">
+      <c r="I278" s="162"/>
+      <c r="J278" s="165">
         <f>J275-D275</f>
         <v>0</v>
       </c>
-      <c r="K278" s="164"/>
+      <c r="K278" s="166"/>
     </row>
     <row r="279" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H279" s="161"/>
-      <c r="I279" s="162"/>
-      <c r="J279" s="165"/>
-      <c r="K279" s="166"/>
+      <c r="H279" s="163"/>
+      <c r="I279" s="164"/>
+      <c r="J279" s="167"/>
+      <c r="K279" s="168"/>
     </row>
     <row r="281" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="282" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D282" s="156" t="s">
+      <c r="D282" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E282" s="157"/>
-      <c r="F282" s="167"/>
-      <c r="G282" s="168"/>
+      <c r="E282" s="159"/>
+      <c r="F282" s="169"/>
+      <c r="G282" s="170"/>
     </row>
     <row r="283" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D283" s="158"/>
-      <c r="E283" s="159"/>
-      <c r="F283" s="169"/>
-      <c r="G283" s="170"/>
+      <c r="D283" s="160"/>
+      <c r="E283" s="161"/>
+      <c r="F283" s="171"/>
+      <c r="G283" s="172"/>
     </row>
     <row r="284" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="285" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D285" s="156" t="s">
+      <c r="D285" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E285" s="157"/>
-      <c r="F285" s="171">
+      <c r="E285" s="159"/>
+      <c r="F285" s="173">
         <f>J278*F282</f>
         <v>0</v>
       </c>
-      <c r="G285" s="172"/>
+      <c r="G285" s="174"/>
     </row>
     <row r="286" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D286" s="158"/>
-      <c r="E286" s="159"/>
-      <c r="F286" s="173"/>
-      <c r="G286" s="174"/>
+      <c r="D286" s="160"/>
+      <c r="E286" s="161"/>
+      <c r="F286" s="175"/>
+      <c r="G286" s="176"/>
     </row>
     <row r="287" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="288" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D288" s="156" t="s">
+      <c r="D288" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E288" s="157"/>
-      <c r="F288" s="156" t="e">
+      <c r="E288" s="159"/>
+      <c r="F288" s="158" t="e">
         <f>J278/H275</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G288" s="157"/>
+      <c r="G288" s="159"/>
     </row>
     <row r="289" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D289" s="158"/>
-      <c r="E289" s="159"/>
-      <c r="F289" s="158"/>
-      <c r="G289" s="159"/>
+      <c r="D289" s="160"/>
+      <c r="E289" s="161"/>
+      <c r="F289" s="160"/>
+      <c r="G289" s="161"/>
     </row>
     <row r="296" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="297" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B297" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C297" s="175"/>
-      <c r="D297" s="176"/>
+      <c r="C297" s="177"/>
+      <c r="D297" s="178"/>
       <c r="F297" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G297" s="177"/>
-      <c r="H297" s="178"/>
+      <c r="G297" s="179"/>
+      <c r="H297" s="180"/>
       <c r="J297" s="11" t="s">
         <v>39</v>
       </c>
@@ -7458,15 +7480,15 @@
     </row>
     <row r="298" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="299" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C299" s="78" t="s">
+      <c r="C299" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D299" s="83"/>
-      <c r="F299" s="156" t="s">
+      <c r="D299" s="85"/>
+      <c r="F299" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G299" s="179"/>
-      <c r="H299" s="157"/>
+      <c r="G299" s="181"/>
+      <c r="H299" s="159"/>
       <c r="J299" s="11" t="s">
         <v>42</v>
       </c>
@@ -7712,85 +7734,85 @@
     </row>
     <row r="318" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="319" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H319" s="156" t="s">
+      <c r="H319" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I319" s="160"/>
-      <c r="J319" s="163">
+      <c r="I319" s="162"/>
+      <c r="J319" s="165">
         <f>J316-D316</f>
         <v>0</v>
       </c>
-      <c r="K319" s="164"/>
+      <c r="K319" s="166"/>
     </row>
     <row r="320" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H320" s="161"/>
-      <c r="I320" s="162"/>
-      <c r="J320" s="165"/>
-      <c r="K320" s="166"/>
+      <c r="H320" s="163"/>
+      <c r="I320" s="164"/>
+      <c r="J320" s="167"/>
+      <c r="K320" s="168"/>
     </row>
     <row r="322" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="323" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D323" s="156" t="s">
+      <c r="D323" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E323" s="157"/>
-      <c r="F323" s="167"/>
-      <c r="G323" s="168"/>
+      <c r="E323" s="159"/>
+      <c r="F323" s="169"/>
+      <c r="G323" s="170"/>
     </row>
     <row r="324" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D324" s="158"/>
-      <c r="E324" s="159"/>
-      <c r="F324" s="169"/>
-      <c r="G324" s="170"/>
+      <c r="D324" s="160"/>
+      <c r="E324" s="161"/>
+      <c r="F324" s="171"/>
+      <c r="G324" s="172"/>
     </row>
     <row r="325" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="326" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D326" s="156" t="s">
+      <c r="D326" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E326" s="157"/>
-      <c r="F326" s="171">
+      <c r="E326" s="159"/>
+      <c r="F326" s="173">
         <f>J319*F323</f>
         <v>0</v>
       </c>
-      <c r="G326" s="172"/>
+      <c r="G326" s="174"/>
     </row>
     <row r="327" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D327" s="158"/>
-      <c r="E327" s="159"/>
-      <c r="F327" s="173"/>
-      <c r="G327" s="174"/>
+      <c r="D327" s="160"/>
+      <c r="E327" s="161"/>
+      <c r="F327" s="175"/>
+      <c r="G327" s="176"/>
     </row>
     <row r="328" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="329" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D329" s="156" t="s">
+      <c r="D329" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E329" s="157"/>
-      <c r="F329" s="156" t="e">
+      <c r="E329" s="159"/>
+      <c r="F329" s="158" t="e">
         <f>J319/H316</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G329" s="157"/>
+      <c r="G329" s="159"/>
     </row>
     <row r="330" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D330" s="158"/>
-      <c r="E330" s="159"/>
-      <c r="F330" s="158"/>
-      <c r="G330" s="159"/>
+      <c r="D330" s="160"/>
+      <c r="E330" s="161"/>
+      <c r="F330" s="160"/>
+      <c r="G330" s="161"/>
     </row>
     <row r="337" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="338" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B338" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C338" s="175"/>
-      <c r="D338" s="176"/>
+      <c r="C338" s="177"/>
+      <c r="D338" s="178"/>
       <c r="F338" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G338" s="177"/>
-      <c r="H338" s="178"/>
+      <c r="G338" s="179"/>
+      <c r="H338" s="180"/>
       <c r="J338" s="11" t="s">
         <v>39</v>
       </c>
@@ -7798,15 +7820,15 @@
     </row>
     <row r="339" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="340" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C340" s="78" t="s">
+      <c r="C340" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D340" s="83"/>
-      <c r="F340" s="156" t="s">
+      <c r="D340" s="85"/>
+      <c r="F340" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G340" s="179"/>
-      <c r="H340" s="157"/>
+      <c r="G340" s="181"/>
+      <c r="H340" s="159"/>
       <c r="J340" s="11" t="s">
         <v>42</v>
       </c>
@@ -8052,85 +8074,85 @@
     </row>
     <row r="359" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="360" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H360" s="156" t="s">
+      <c r="H360" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I360" s="160"/>
-      <c r="J360" s="163">
+      <c r="I360" s="162"/>
+      <c r="J360" s="165">
         <f>J357-D357</f>
         <v>0</v>
       </c>
-      <c r="K360" s="164"/>
+      <c r="K360" s="166"/>
     </row>
     <row r="361" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H361" s="161"/>
-      <c r="I361" s="162"/>
-      <c r="J361" s="165"/>
-      <c r="K361" s="166"/>
+      <c r="H361" s="163"/>
+      <c r="I361" s="164"/>
+      <c r="J361" s="167"/>
+      <c r="K361" s="168"/>
     </row>
     <row r="363" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="364" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D364" s="156" t="s">
+      <c r="D364" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E364" s="157"/>
-      <c r="F364" s="167"/>
-      <c r="G364" s="168"/>
+      <c r="E364" s="159"/>
+      <c r="F364" s="169"/>
+      <c r="G364" s="170"/>
     </row>
     <row r="365" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D365" s="158"/>
-      <c r="E365" s="159"/>
-      <c r="F365" s="169"/>
-      <c r="G365" s="170"/>
+      <c r="D365" s="160"/>
+      <c r="E365" s="161"/>
+      <c r="F365" s="171"/>
+      <c r="G365" s="172"/>
     </row>
     <row r="366" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="367" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D367" s="156" t="s">
+      <c r="D367" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E367" s="157"/>
-      <c r="F367" s="171">
+      <c r="E367" s="159"/>
+      <c r="F367" s="173">
         <f>J360*F364</f>
         <v>0</v>
       </c>
-      <c r="G367" s="172"/>
+      <c r="G367" s="174"/>
     </row>
     <row r="368" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D368" s="158"/>
-      <c r="E368" s="159"/>
-      <c r="F368" s="173"/>
-      <c r="G368" s="174"/>
+      <c r="D368" s="160"/>
+      <c r="E368" s="161"/>
+      <c r="F368" s="175"/>
+      <c r="G368" s="176"/>
     </row>
     <row r="369" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="370" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D370" s="156" t="s">
+      <c r="D370" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E370" s="157"/>
-      <c r="F370" s="156" t="e">
+      <c r="E370" s="159"/>
+      <c r="F370" s="158" t="e">
         <f>J360/H357</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G370" s="157"/>
+      <c r="G370" s="159"/>
     </row>
     <row r="371" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D371" s="158"/>
-      <c r="E371" s="159"/>
-      <c r="F371" s="158"/>
-      <c r="G371" s="159"/>
+      <c r="D371" s="160"/>
+      <c r="E371" s="161"/>
+      <c r="F371" s="160"/>
+      <c r="G371" s="161"/>
     </row>
     <row r="378" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="379" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B379" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C379" s="175"/>
-      <c r="D379" s="176"/>
+      <c r="C379" s="177"/>
+      <c r="D379" s="178"/>
       <c r="F379" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G379" s="177"/>
-      <c r="H379" s="178"/>
+      <c r="G379" s="179"/>
+      <c r="H379" s="180"/>
       <c r="J379" s="11" t="s">
         <v>39</v>
       </c>
@@ -8138,15 +8160,15 @@
     </row>
     <row r="380" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="381" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C381" s="78" t="s">
+      <c r="C381" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D381" s="83"/>
-      <c r="F381" s="156" t="s">
+      <c r="D381" s="85"/>
+      <c r="F381" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G381" s="179"/>
-      <c r="H381" s="157"/>
+      <c r="G381" s="181"/>
+      <c r="H381" s="159"/>
       <c r="J381" s="11" t="s">
         <v>42</v>
       </c>
@@ -8392,85 +8414,85 @@
     </row>
     <row r="400" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="401" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="H401" s="156" t="s">
+      <c r="H401" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I401" s="160"/>
-      <c r="J401" s="163">
+      <c r="I401" s="162"/>
+      <c r="J401" s="165">
         <f>J398-D398</f>
         <v>0</v>
       </c>
-      <c r="K401" s="164"/>
+      <c r="K401" s="166"/>
     </row>
     <row r="402" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H402" s="161"/>
-      <c r="I402" s="162"/>
-      <c r="J402" s="165"/>
-      <c r="K402" s="166"/>
+      <c r="H402" s="163"/>
+      <c r="I402" s="164"/>
+      <c r="J402" s="167"/>
+      <c r="K402" s="168"/>
     </row>
     <row r="404" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="405" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D405" s="156" t="s">
+      <c r="D405" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E405" s="157"/>
-      <c r="F405" s="167"/>
-      <c r="G405" s="168"/>
+      <c r="E405" s="159"/>
+      <c r="F405" s="169"/>
+      <c r="G405" s="170"/>
     </row>
     <row r="406" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D406" s="158"/>
-      <c r="E406" s="159"/>
-      <c r="F406" s="169"/>
-      <c r="G406" s="170"/>
+      <c r="D406" s="160"/>
+      <c r="E406" s="161"/>
+      <c r="F406" s="171"/>
+      <c r="G406" s="172"/>
     </row>
     <row r="407" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="408" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D408" s="156" t="s">
+      <c r="D408" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E408" s="157"/>
-      <c r="F408" s="171">
+      <c r="E408" s="159"/>
+      <c r="F408" s="173">
         <f>J401*F405</f>
         <v>0</v>
       </c>
-      <c r="G408" s="172"/>
+      <c r="G408" s="174"/>
     </row>
     <row r="409" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D409" s="158"/>
-      <c r="E409" s="159"/>
-      <c r="F409" s="173"/>
-      <c r="G409" s="174"/>
+      <c r="D409" s="160"/>
+      <c r="E409" s="161"/>
+      <c r="F409" s="175"/>
+      <c r="G409" s="176"/>
     </row>
     <row r="410" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="411" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D411" s="156" t="s">
+      <c r="D411" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E411" s="157"/>
-      <c r="F411" s="156" t="e">
+      <c r="E411" s="159"/>
+      <c r="F411" s="158" t="e">
         <f>J401/H398</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G411" s="157"/>
+      <c r="G411" s="159"/>
     </row>
     <row r="412" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D412" s="158"/>
-      <c r="E412" s="159"/>
-      <c r="F412" s="158"/>
-      <c r="G412" s="159"/>
+      <c r="D412" s="160"/>
+      <c r="E412" s="161"/>
+      <c r="F412" s="160"/>
+      <c r="G412" s="161"/>
     </row>
     <row r="419" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="420" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B420" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C420" s="175"/>
-      <c r="D420" s="176"/>
+      <c r="C420" s="177"/>
+      <c r="D420" s="178"/>
       <c r="F420" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G420" s="177"/>
-      <c r="H420" s="178"/>
+      <c r="G420" s="179"/>
+      <c r="H420" s="180"/>
       <c r="J420" s="11" t="s">
         <v>39</v>
       </c>
@@ -8478,15 +8500,15 @@
     </row>
     <row r="421" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="422" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C422" s="78" t="s">
+      <c r="C422" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D422" s="83"/>
-      <c r="F422" s="156" t="s">
+      <c r="D422" s="85"/>
+      <c r="F422" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G422" s="179"/>
-      <c r="H422" s="157"/>
+      <c r="G422" s="181"/>
+      <c r="H422" s="159"/>
       <c r="J422" s="11" t="s">
         <v>42</v>
       </c>
@@ -8732,85 +8754,85 @@
     </row>
     <row r="441" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="442" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H442" s="156" t="s">
+      <c r="H442" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I442" s="160"/>
-      <c r="J442" s="163">
+      <c r="I442" s="162"/>
+      <c r="J442" s="165">
         <f>J439-D439</f>
         <v>0</v>
       </c>
-      <c r="K442" s="164"/>
+      <c r="K442" s="166"/>
     </row>
     <row r="443" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H443" s="161"/>
-      <c r="I443" s="162"/>
-      <c r="J443" s="165"/>
-      <c r="K443" s="166"/>
+      <c r="H443" s="163"/>
+      <c r="I443" s="164"/>
+      <c r="J443" s="167"/>
+      <c r="K443" s="168"/>
     </row>
     <row r="445" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="446" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D446" s="156" t="s">
+      <c r="D446" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E446" s="157"/>
-      <c r="F446" s="167"/>
-      <c r="G446" s="168"/>
+      <c r="E446" s="159"/>
+      <c r="F446" s="169"/>
+      <c r="G446" s="170"/>
     </row>
     <row r="447" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D447" s="158"/>
-      <c r="E447" s="159"/>
-      <c r="F447" s="169"/>
-      <c r="G447" s="170"/>
+      <c r="D447" s="160"/>
+      <c r="E447" s="161"/>
+      <c r="F447" s="171"/>
+      <c r="G447" s="172"/>
     </row>
     <row r="448" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="449" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D449" s="156" t="s">
+      <c r="D449" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E449" s="157"/>
-      <c r="F449" s="171">
+      <c r="E449" s="159"/>
+      <c r="F449" s="173">
         <f>J442*F446</f>
         <v>0</v>
       </c>
-      <c r="G449" s="172"/>
+      <c r="G449" s="174"/>
     </row>
     <row r="450" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D450" s="158"/>
-      <c r="E450" s="159"/>
-      <c r="F450" s="173"/>
-      <c r="G450" s="174"/>
+      <c r="D450" s="160"/>
+      <c r="E450" s="161"/>
+      <c r="F450" s="175"/>
+      <c r="G450" s="176"/>
     </row>
     <row r="451" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="452" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D452" s="156" t="s">
+      <c r="D452" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E452" s="157"/>
-      <c r="F452" s="156" t="e">
+      <c r="E452" s="159"/>
+      <c r="F452" s="158" t="e">
         <f>J442/H439</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G452" s="157"/>
+      <c r="G452" s="159"/>
     </row>
     <row r="453" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D453" s="158"/>
-      <c r="E453" s="159"/>
-      <c r="F453" s="158"/>
-      <c r="G453" s="159"/>
+      <c r="D453" s="160"/>
+      <c r="E453" s="161"/>
+      <c r="F453" s="160"/>
+      <c r="G453" s="161"/>
     </row>
     <row r="460" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="461" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B461" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C461" s="175"/>
-      <c r="D461" s="176"/>
+      <c r="C461" s="177"/>
+      <c r="D461" s="178"/>
       <c r="F461" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G461" s="177"/>
-      <c r="H461" s="178"/>
+      <c r="G461" s="179"/>
+      <c r="H461" s="180"/>
       <c r="J461" s="11" t="s">
         <v>39</v>
       </c>
@@ -8818,15 +8840,15 @@
     </row>
     <row r="462" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="463" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C463" s="78" t="s">
+      <c r="C463" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D463" s="83"/>
-      <c r="F463" s="156" t="s">
+      <c r="D463" s="85"/>
+      <c r="F463" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="G463" s="179"/>
-      <c r="H463" s="157"/>
+      <c r="G463" s="181"/>
+      <c r="H463" s="159"/>
       <c r="J463" s="11" t="s">
         <v>42</v>
       </c>
@@ -9072,72 +9094,72 @@
     </row>
     <row r="482" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="483" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="H483" s="156" t="s">
+      <c r="H483" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="I483" s="160"/>
-      <c r="J483" s="163">
+      <c r="I483" s="162"/>
+      <c r="J483" s="165">
         <f>J480-D480</f>
         <v>0</v>
       </c>
-      <c r="K483" s="164"/>
+      <c r="K483" s="166"/>
     </row>
     <row r="484" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H484" s="161"/>
-      <c r="I484" s="162"/>
-      <c r="J484" s="165"/>
-      <c r="K484" s="166"/>
+      <c r="H484" s="163"/>
+      <c r="I484" s="164"/>
+      <c r="J484" s="167"/>
+      <c r="K484" s="168"/>
     </row>
     <row r="486" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="487" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D487" s="156" t="s">
+      <c r="D487" s="158" t="s">
         <v>50</v>
       </c>
-      <c r="E487" s="157"/>
-      <c r="F487" s="167"/>
-      <c r="G487" s="168"/>
+      <c r="E487" s="159"/>
+      <c r="F487" s="169"/>
+      <c r="G487" s="170"/>
     </row>
     <row r="488" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D488" s="158"/>
-      <c r="E488" s="159"/>
-      <c r="F488" s="169"/>
-      <c r="G488" s="170"/>
+      <c r="D488" s="160"/>
+      <c r="E488" s="161"/>
+      <c r="F488" s="171"/>
+      <c r="G488" s="172"/>
     </row>
     <row r="489" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="490" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D490" s="156" t="s">
+      <c r="D490" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="E490" s="157"/>
-      <c r="F490" s="171">
+      <c r="E490" s="159"/>
+      <c r="F490" s="173">
         <f>J483*F487</f>
         <v>0</v>
       </c>
-      <c r="G490" s="172"/>
+      <c r="G490" s="174"/>
     </row>
     <row r="491" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D491" s="158"/>
-      <c r="E491" s="159"/>
-      <c r="F491" s="173"/>
-      <c r="G491" s="174"/>
+      <c r="D491" s="160"/>
+      <c r="E491" s="161"/>
+      <c r="F491" s="175"/>
+      <c r="G491" s="176"/>
     </row>
     <row r="492" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="493" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D493" s="156" t="s">
+      <c r="D493" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="E493" s="157"/>
-      <c r="F493" s="156" t="e">
+      <c r="E493" s="159"/>
+      <c r="F493" s="158" t="e">
         <f>J483/H480</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G493" s="157"/>
+      <c r="G493" s="159"/>
     </row>
     <row r="494" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D494" s="158"/>
-      <c r="E494" s="159"/>
-      <c r="F494" s="158"/>
-      <c r="G494" s="159"/>
+      <c r="D494" s="160"/>
+      <c r="E494" s="161"/>
+      <c r="F494" s="160"/>
+      <c r="G494" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="164">
@@ -9155,6 +9177,8 @@
     <mergeCell ref="E203:E204"/>
     <mergeCell ref="D205:D207"/>
     <mergeCell ref="E205:E207"/>
+    <mergeCell ref="F203:F204"/>
+    <mergeCell ref="F205:F207"/>
     <mergeCell ref="D148:E149"/>
     <mergeCell ref="F148:G149"/>
     <mergeCell ref="D151:E152"/>
@@ -9202,8 +9226,6 @@
     <mergeCell ref="F30:G31"/>
     <mergeCell ref="D33:E34"/>
     <mergeCell ref="F33:G34"/>
-    <mergeCell ref="F203:F204"/>
-    <mergeCell ref="F205:F207"/>
     <mergeCell ref="K202:K204"/>
     <mergeCell ref="K205:K207"/>
     <mergeCell ref="L202:L204"/>
@@ -9309,4 +9331,313 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5047D52-5EDF-449D-A17A-EE491592BE6D}">
+  <dimension ref="B2:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
+        <f>SALES!G4</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="52">
+        <f>SALES!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <f>SALES!F33</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <f>IF(OR(ISBLANK(F3),F3="Not Paid"),D3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="8">
+        <f>SALES!G43</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="52">
+        <f>SALES!C43</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <f>SALES!F72</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" ref="E4:E14" si="0">IF(OR(ISBLANK(F4),F4="Not Paid"),D4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="8">
+        <f>SALES!G83</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="52">
+        <f>SALES!C83</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <f>SALES!F112</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="8">
+        <f>SALES!G122</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="52">
+        <f>SALES!C122</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <f>SALES!F151</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="8">
+        <f>SALES!G163</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="52">
+        <f>SALES!C163</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <f>SALES!F192</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="8">
+        <f>SALES!G215</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="52">
+        <f>SALES!C215</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <f>SALES!F244</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="8">
+        <f>SALES!G256</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="52">
+        <f>SALES!C256</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <f>SALES!F285</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="8">
+        <f>SALES!G297</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="52">
+        <f>SALES!C297</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <f>SALES!F326</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="8">
+        <f>SALES!G338</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="52">
+        <f>SALES!C338</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <f>SALES!F367</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="8">
+        <f>SALES!G379</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="52">
+        <f>SALES!C379</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <f>SALES!F408</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="8">
+        <f>SALES!G420</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="52">
+        <f>SALES!C420</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <f>SALES!F449</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="8">
+        <f>SALES!G461</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="52">
+        <f>SALES!C461</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <f>SALES!F490</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="143" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="158">
+        <f>SUM(E3:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="181"/>
+      <c r="E17" s="159"/>
+    </row>
+    <row r="18" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="145"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="186"/>
+      <c r="E18" s="161"/>
+    </row>
+    <row r="21" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="143" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="158">
+        <f>SUM(D3:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="181"/>
+      <c r="E22" s="159"/>
+    </row>
+    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="145"/>
+      <c r="C23" s="160"/>
+      <c r="D23" s="186"/>
+      <c r="E23" s="161"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:E18"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:E23"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F14" xr:uid="{E215E107-6E57-4A98-A477-B92F13F99DC5}">
+      <formula1>"Not Paid, Paid"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added file salary of employee And edit in payment pending in joseph Poultry
</commit_message>
<xml_diff>
--- a/JOSEPH Poultry.xlsx
+++ b/JOSEPH Poultry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KUREETHADOM\Common\Poultry Farm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KUREETHADOM\Common\Poultry Farm\RawFile\Version 3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8229F3E4-68C9-42A3-A4D8-465293B68ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9125C5-F42B-42E6-B530-32A804A88107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="420" windowWidth="12240" windowHeight="11820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHICKS" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,12 @@
     <sheet name="SALES" sheetId="3" r:id="rId3"/>
     <sheet name="Pending Payment" sheetId="5" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="82">
   <si>
     <t>Date of Arrival</t>
   </si>
@@ -270,6 +267,9 @@
   <si>
     <t>Pending</t>
   </si>
+  <si>
+    <t>Paid</t>
+  </si>
 </sst>
 </file>
 
@@ -1642,49 +1642,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="CHICKS"/>
-      <sheetName val="EXPENSE"/>
-      <sheetName val="SALES"/>
-      <sheetName val="Pending Payment"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="20">
-          <cell r="J20">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="78">
-          <cell r="G78">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="205">
-          <cell r="B205">
-            <v>0</v>
-          </cell>
-          <cell r="D205">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1977,7 +1934,7 @@
   <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G3"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3508,7 +3465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F79CD94-4843-44B4-9F4B-EBB62E1DDF57}">
   <dimension ref="A2:O83"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="97" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A58" zoomScale="97" workbookViewId="0">
+      <selection activeCell="R74" sqref="R74"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4957,8 +4916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06126A5B-91A0-41E1-A06A-A0919D230834}">
   <dimension ref="B3:P494"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="C205" sqref="C205:C207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6727,7 +6686,7 @@
         <v>0</v>
       </c>
       <c r="C205" s="53">
-        <f>[1]CHICKS!J20-[1]SALES!B205</f>
+        <f>CHICKS!J20-SALES!B205</f>
         <v>0</v>
       </c>
       <c r="D205" s="53">
@@ -6735,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="E205" s="53">
-        <f>[1]SALES!D205-[1]EXPENSE!G78</f>
+        <f>SALES!D205-EXPENSE!G78</f>
         <v>0</v>
       </c>
       <c r="F205" s="53">
@@ -9335,15 +9294,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5047D52-5EDF-449D-A17A-EE491592BE6D}">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="51" t="s">
         <v>3</v>
       </c>
@@ -9359,8 +9318,11 @@
       <c r="F2" s="51" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="8">
         <f>SALES!G4</f>
         <v>0</v>
@@ -9374,14 +9336,15 @@
         <v>0</v>
       </c>
       <c r="E3" s="7">
-        <f>IF(OR(ISBLANK(F3),F3="Not Paid"),D3,0)</f>
+        <f>IF(OR(ISBLANK(F3),F3="Not Paid"),D3,0)-G3</f>
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="8">
         <f>SALES!G43</f>
         <v>0</v>
@@ -9395,12 +9358,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="7">
-        <f t="shared" ref="E4:E14" si="0">IF(OR(ISBLANK(F4),F4="Not Paid"),D4,0)</f>
+        <f>IF(OR(ISBLANK(F4),F4="Not Paid"),D4,0)-G4</f>
         <v>0</v>
       </c>
       <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
         <f>SALES!G83</f>
         <v>0</v>
@@ -9414,12 +9378,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" si="0"/>
+        <f>IF(OR(ISBLANK(F5),F5="Not Paid"),D5,0)-G5</f>
         <v>0</v>
       </c>
       <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="8">
         <f>SALES!G122</f>
         <v>0</v>
@@ -9433,12 +9398,13 @@
         <v>0</v>
       </c>
       <c r="E6" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E6:E14" si="0">IF(OR(ISBLANK(F6),F6="Not Paid"),D6,0)-G6</f>
         <v>0</v>
       </c>
       <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <f>SALES!G163</f>
         <v>0</v>
@@ -9456,8 +9422,9 @@
         <v>0</v>
       </c>
       <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="8">
         <f>SALES!G215</f>
         <v>0</v>
@@ -9475,8 +9442,9 @@
         <v>0</v>
       </c>
       <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="8">
         <f>SALES!G256</f>
         <v>0</v>
@@ -9494,8 +9462,9 @@
         <v>0</v>
       </c>
       <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <f>SALES!G297</f>
         <v>0</v>
@@ -9513,8 +9482,9 @@
         <v>0</v>
       </c>
       <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <f>SALES!G338</f>
         <v>0</v>
@@ -9532,8 +9502,9 @@
         <v>0</v>
       </c>
       <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="8">
         <f>SALES!G379</f>
         <v>0</v>
@@ -9551,8 +9522,9 @@
         <v>0</v>
       </c>
       <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="8">
         <f>SALES!G420</f>
         <v>0</v>
@@ -9570,8 +9542,9 @@
         <v>0</v>
       </c>
       <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <f>SALES!G461</f>
         <v>0</v>
@@ -9589,8 +9562,9 @@
         <v>0</v>
       </c>
       <c r="F14" s="7"/>
-    </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="16" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="143" t="s">
         <v>80</v>

</xml_diff>